<commit_message>
Read exactresults from SAF
</commit_message>
<xml_diff>
--- a/backend/analysis/annotations/test_files/sample_16_SAF.xlsx
+++ b/backend/analysis/annotations/test_files/sample_16_SAF.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X323"/>
+  <dimension ref="A1:X330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="F65" s="2" t="inlineStr">
         <is>
-          <t>Breda</t>
+          <t>breda</t>
         </is>
       </c>
       <c r="G65" s="2" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="G93" s="2" t="inlineStr">
         <is>
-          <t>ZORGINSTELLING1</t>
+          <t>zorginstelling1</t>
         </is>
       </c>
       <c r="H93" s="2" t="n"/>
@@ -4407,7 +4407,7 @@
       </c>
       <c r="D100" s="2" t="inlineStr">
         <is>
-          <t>BEROEP1</t>
+          <t>beroep1</t>
         </is>
       </c>
       <c r="E100" s="2" t="n"/>
@@ -9011,7 +9011,7 @@
       </c>
       <c r="H219" s="2" t="inlineStr">
         <is>
-          <t>WERKINSTELLING1</t>
+          <t>werkinstelling1</t>
         </is>
       </c>
       <c r="I219" s="2" t="n"/>
@@ -10782,7 +10782,7 @@
       </c>
       <c r="C268" s="2" t="inlineStr">
         <is>
-          <t>WERKINSTELLING2</t>
+          <t>werkinstelling2</t>
         </is>
       </c>
       <c r="D268" s="2" t="n"/>
@@ -11778,64 +11778,24 @@
       </c>
       <c r="C296" s="2" t="inlineStr">
         <is>
-          <t>dus</t>
+          <t>ik</t>
         </is>
       </c>
       <c r="D296" s="2" t="inlineStr">
         <is>
-          <t>maar</t>
-        </is>
-      </c>
-      <c r="E296" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="F296" s="2" t="inlineStr">
-        <is>
-          <t>ik</t>
-        </is>
-      </c>
-      <c r="G296" s="2" t="inlineStr">
-        <is>
-          <t>veel</t>
-        </is>
-      </c>
-      <c r="H296" s="2" t="inlineStr">
-        <is>
-          <t>geweest</t>
-        </is>
-      </c>
-      <c r="I296" s="2" t="inlineStr">
-        <is>
-          <t>maar</t>
-        </is>
-      </c>
-      <c r="J296" s="2" t="inlineStr">
-        <is>
-          <t>ook</t>
-        </is>
-      </c>
-      <c r="K296" s="2" t="inlineStr">
-        <is>
-          <t>als</t>
-        </is>
-      </c>
-      <c r="L296" s="2" t="inlineStr">
-        <is>
-          <t>ik</t>
-        </is>
-      </c>
-      <c r="M296" s="2" t="inlineStr">
-        <is>
-          <t>hier</t>
-        </is>
-      </c>
-      <c r="N296" s="2" t="inlineStr">
-        <is>
-          <t>uh</t>
-        </is>
-      </c>
+          <t>weet</t>
+        </is>
+      </c>
+      <c r="E296" s="2" t="n"/>
+      <c r="F296" s="2" t="n"/>
+      <c r="G296" s="2" t="n"/>
+      <c r="H296" s="2" t="n"/>
+      <c r="I296" s="2" t="n"/>
+      <c r="J296" s="2" t="n"/>
+      <c r="K296" s="2" t="n"/>
+      <c r="L296" s="2" t="n"/>
+      <c r="M296" s="2" t="n"/>
+      <c r="N296" s="2" t="n"/>
       <c r="O296" s="2" t="n"/>
       <c r="P296" s="2" t="n"/>
       <c r="Q296" s="2" t="n"/>
@@ -11867,11 +11827,7 @@
       <c r="K297" s="3" t="n"/>
       <c r="L297" s="3" t="n"/>
       <c r="M297" s="3" t="n"/>
-      <c r="N297" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="N297" s="3" t="n"/>
       <c r="O297" s="3" t="n"/>
       <c r="P297" s="3" t="n"/>
       <c r="Q297" s="3" t="n"/>
@@ -11925,19 +11881,15 @@
         </is>
       </c>
       <c r="C299" s="3" t="n"/>
-      <c r="D299" s="3" t="n"/>
-      <c r="E299" s="3" t="inlineStr">
-        <is>
-          <t>PV</t>
-        </is>
-      </c>
+      <c r="D299" s="3" t="inlineStr">
+        <is>
+          <t>LEX,PV</t>
+        </is>
+      </c>
+      <c r="E299" s="3" t="n"/>
       <c r="F299" s="3" t="n"/>
       <c r="G299" s="3" t="n"/>
-      <c r="H299" s="3" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
+      <c r="H299" s="3" t="n"/>
       <c r="I299" s="3" t="n"/>
       <c r="J299" s="3" t="n"/>
       <c r="K299" s="3" t="n"/>
@@ -12062,57 +12014,57 @@
       </c>
       <c r="C303" s="2" t="inlineStr">
         <is>
-          <t>oo</t>
+          <t>dus</t>
         </is>
       </c>
       <c r="D303" s="2" t="inlineStr">
         <is>
-          <t>uh</t>
+          <t>maar</t>
         </is>
       </c>
       <c r="E303" s="2" t="inlineStr">
         <is>
-          <t>ja</t>
+          <t>ben</t>
         </is>
       </c>
       <c r="F303" s="2" t="inlineStr">
         <is>
-          <t>uh</t>
+          <t>ik</t>
         </is>
       </c>
       <c r="G303" s="2" t="inlineStr">
         <is>
-          <t>uh</t>
+          <t>veel</t>
         </is>
       </c>
       <c r="H303" s="2" t="inlineStr">
         <is>
+          <t>geweest</t>
+        </is>
+      </c>
+      <c r="I303" s="2" t="inlineStr">
+        <is>
+          <t>maar</t>
+        </is>
+      </c>
+      <c r="J303" s="2" t="inlineStr">
+        <is>
+          <t>ook</t>
+        </is>
+      </c>
+      <c r="K303" s="2" t="inlineStr">
+        <is>
+          <t>als</t>
+        </is>
+      </c>
+      <c r="L303" s="2" t="inlineStr">
+        <is>
           <t>ik</t>
         </is>
       </c>
-      <c r="I303" s="2" t="inlineStr">
-        <is>
-          <t>zing</t>
-        </is>
-      </c>
-      <c r="J303" s="2" t="inlineStr">
-        <is>
-          <t>met</t>
-        </is>
-      </c>
-      <c r="K303" s="2" t="inlineStr">
-        <is>
-          <t>uh</t>
-        </is>
-      </c>
-      <c r="L303" s="2" t="inlineStr">
-        <is>
-          <t>oudere</t>
-        </is>
-      </c>
       <c r="M303" s="2" t="inlineStr">
         <is>
-          <t>mensen</t>
+          <t>hier</t>
         </is>
       </c>
       <c r="N303" s="2" t="inlineStr">
@@ -12140,35 +12092,15 @@
           <t>SampleGrootte</t>
         </is>
       </c>
-      <c r="C304" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="D304" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="C304" s="3" t="n"/>
+      <c r="D304" s="3" t="n"/>
       <c r="E304" s="3" t="n"/>
-      <c r="F304" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G304" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="F304" s="3" t="n"/>
+      <c r="G304" s="3" t="n"/>
       <c r="H304" s="3" t="n"/>
       <c r="I304" s="3" t="n"/>
       <c r="J304" s="3" t="n"/>
-      <c r="K304" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="K304" s="3" t="n"/>
       <c r="L304" s="3" t="n"/>
       <c r="M304" s="3" t="n"/>
       <c r="N304" s="3" t="inlineStr">
@@ -12198,11 +12130,7 @@
       </c>
       <c r="C305" s="3" t="n"/>
       <c r="D305" s="3" t="n"/>
-      <c r="E305" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="E305" s="3" t="n"/>
       <c r="F305" s="3" t="n"/>
       <c r="G305" s="3" t="n"/>
       <c r="H305" s="3" t="n"/>
@@ -12234,27 +12162,23 @@
       </c>
       <c r="C306" s="3" t="n"/>
       <c r="D306" s="3" t="n"/>
-      <c r="E306" s="3" t="n"/>
+      <c r="E306" s="3" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
       <c r="F306" s="3" t="n"/>
       <c r="G306" s="3" t="n"/>
-      <c r="H306" s="3" t="n"/>
-      <c r="I306" s="3" t="inlineStr">
-        <is>
-          <t>LEX,PV</t>
-        </is>
-      </c>
+      <c r="H306" s="3" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="I306" s="3" t="n"/>
       <c r="J306" s="3" t="n"/>
       <c r="K306" s="3" t="n"/>
-      <c r="L306" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="M306" s="3" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+      <c r="L306" s="3" t="n"/>
+      <c r="M306" s="3" t="n"/>
       <c r="N306" s="3" t="n"/>
       <c r="O306" s="3" t="n"/>
       <c r="P306" s="3" t="n"/>
@@ -12374,69 +12298,65 @@
       </c>
       <c r="C310" s="2" t="inlineStr">
         <is>
+          <t>oo</t>
+        </is>
+      </c>
+      <c r="D310" s="2" t="inlineStr">
+        <is>
+          <t>uh</t>
+        </is>
+      </c>
+      <c r="E310" s="2" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="F310" s="2" t="inlineStr">
+        <is>
+          <t>uh</t>
+        </is>
+      </c>
+      <c r="G310" s="2" t="inlineStr">
+        <is>
+          <t>uh</t>
+        </is>
+      </c>
+      <c r="H310" s="2" t="inlineStr">
+        <is>
           <t>ik</t>
         </is>
       </c>
-      <c r="D310" s="2" t="inlineStr">
+      <c r="I310" s="2" t="inlineStr">
+        <is>
+          <t>zing</t>
+        </is>
+      </c>
+      <c r="J310" s="2" t="inlineStr">
+        <is>
+          <t>met</t>
+        </is>
+      </c>
+      <c r="K310" s="2" t="inlineStr">
         <is>
           <t>uh</t>
         </is>
       </c>
-      <c r="E310" s="2" t="inlineStr">
+      <c r="L310" s="2" t="inlineStr">
+        <is>
+          <t>oudere</t>
+        </is>
+      </c>
+      <c r="M310" s="2" t="inlineStr">
+        <is>
+          <t>mensen</t>
+        </is>
+      </c>
+      <c r="N310" s="2" t="inlineStr">
         <is>
           <t>uh</t>
         </is>
       </c>
-      <c r="F310" s="2" t="inlineStr">
-        <is>
-          <t>ik</t>
-        </is>
-      </c>
-      <c r="G310" s="2" t="inlineStr">
-        <is>
-          <t>doe</t>
-        </is>
-      </c>
-      <c r="H310" s="2" t="inlineStr">
-        <is>
-          <t>uh</t>
-        </is>
-      </c>
-      <c r="I310" s="2" t="inlineStr">
-        <is>
-          <t>boekjes</t>
-        </is>
-      </c>
-      <c r="J310" s="2" t="inlineStr">
-        <is>
-          <t>voor</t>
-        </is>
-      </c>
-      <c r="K310" s="2" t="inlineStr">
-        <is>
-          <t>uh</t>
-        </is>
-      </c>
-      <c r="L310" s="2" t="inlineStr">
-        <is>
-          <t>club</t>
-        </is>
-      </c>
-      <c r="M310" s="2" t="inlineStr">
-        <is>
-          <t>geloof</t>
-        </is>
-      </c>
-      <c r="N310" s="2" t="inlineStr">
-        <is>
-          <t>ik</t>
-        </is>
-      </c>
-      <c r="O310" s="2" t="inlineStr">
-        <is>
-          <t>uh</t>
-        </is>
-      </c>
+      <c r="O310" s="2" t="n"/>
       <c r="P310" s="2" t="n"/>
       <c r="Q310" s="2" t="n"/>
       <c r="R310" s="2" t="n"/>
@@ -12456,24 +12376,28 @@
           <t>SampleGrootte</t>
         </is>
       </c>
-      <c r="C311" s="3" t="n"/>
+      <c r="C311" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D311" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="E311" s="3" t="inlineStr">
+      <c r="E311" s="3" t="n"/>
+      <c r="F311" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="F311" s="3" t="n"/>
-      <c r="G311" s="3" t="n"/>
-      <c r="H311" s="3" t="inlineStr">
+      <c r="G311" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
+      <c r="H311" s="3" t="n"/>
       <c r="I311" s="3" t="n"/>
       <c r="J311" s="3" t="n"/>
       <c r="K311" s="3" t="inlineStr">
@@ -12483,12 +12407,12 @@
       </c>
       <c r="L311" s="3" t="n"/>
       <c r="M311" s="3" t="n"/>
-      <c r="N311" s="3" t="n"/>
-      <c r="O311" s="3" t="inlineStr">
+      <c r="N311" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
+      <c r="O311" s="3" t="n"/>
       <c r="P311" s="3" t="n"/>
       <c r="Q311" s="3" t="n"/>
       <c r="R311" s="3" t="n"/>
@@ -12508,13 +12432,13 @@
           <t>MLU</t>
         </is>
       </c>
-      <c r="C312" s="3" t="inlineStr">
+      <c r="C312" s="3" t="n"/>
+      <c r="D312" s="3" t="n"/>
+      <c r="E312" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D312" s="3" t="n"/>
-      <c r="E312" s="3" t="n"/>
       <c r="F312" s="3" t="n"/>
       <c r="G312" s="3" t="n"/>
       <c r="H312" s="3" t="n"/>
@@ -12548,27 +12472,23 @@
       <c r="D313" s="3" t="n"/>
       <c r="E313" s="3" t="n"/>
       <c r="F313" s="3" t="n"/>
-      <c r="G313" s="3" t="inlineStr">
-        <is>
-          <t>LEX,PV</t>
-        </is>
-      </c>
+      <c r="G313" s="3" t="n"/>
       <c r="H313" s="3" t="n"/>
       <c r="I313" s="3" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>LEX,PV</t>
         </is>
       </c>
       <c r="J313" s="3" t="n"/>
       <c r="K313" s="3" t="n"/>
       <c r="L313" s="3" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="M313" s="3" t="inlineStr">
+        <is>
           <t>N</t>
-        </is>
-      </c>
-      <c r="M313" s="3" t="inlineStr">
-        <is>
-          <t>LEX,PV</t>
         </is>
       </c>
       <c r="N313" s="3" t="n"/>
@@ -12690,7 +12610,7 @@
       </c>
       <c r="C317" s="2" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>ik</t>
         </is>
       </c>
       <c r="D317" s="2" t="inlineStr">
@@ -12705,22 +12625,54 @@
       </c>
       <c r="F317" s="2" t="inlineStr">
         <is>
+          <t>ik</t>
+        </is>
+      </c>
+      <c r="G317" s="2" t="inlineStr">
+        <is>
+          <t>doe</t>
+        </is>
+      </c>
+      <c r="H317" s="2" t="inlineStr">
+        <is>
           <t>uh</t>
         </is>
       </c>
-      <c r="G317" s="2" t="inlineStr">
-        <is>
-          <t>sorry</t>
-        </is>
-      </c>
-      <c r="H317" s="2" t="n"/>
-      <c r="I317" s="2" t="n"/>
-      <c r="J317" s="2" t="n"/>
-      <c r="K317" s="2" t="n"/>
-      <c r="L317" s="2" t="n"/>
-      <c r="M317" s="2" t="n"/>
-      <c r="N317" s="2" t="n"/>
-      <c r="O317" s="2" t="n"/>
+      <c r="I317" s="2" t="inlineStr">
+        <is>
+          <t>boekjes</t>
+        </is>
+      </c>
+      <c r="J317" s="2" t="inlineStr">
+        <is>
+          <t>voor</t>
+        </is>
+      </c>
+      <c r="K317" s="2" t="inlineStr">
+        <is>
+          <t>uh</t>
+        </is>
+      </c>
+      <c r="L317" s="2" t="inlineStr">
+        <is>
+          <t>club</t>
+        </is>
+      </c>
+      <c r="M317" s="2" t="inlineStr">
+        <is>
+          <t>geloof</t>
+        </is>
+      </c>
+      <c r="N317" s="2" t="inlineStr">
+        <is>
+          <t>ik</t>
+        </is>
+      </c>
+      <c r="O317" s="2" t="inlineStr">
+        <is>
+          <t>uh</t>
+        </is>
+      </c>
       <c r="P317" s="2" t="n"/>
       <c r="Q317" s="2" t="n"/>
       <c r="R317" s="2" t="n"/>
@@ -12751,24 +12703,28 @@
           <t>X</t>
         </is>
       </c>
-      <c r="F318" s="3" t="inlineStr">
+      <c r="F318" s="3" t="n"/>
+      <c r="G318" s="3" t="n"/>
+      <c r="H318" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="G318" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H318" s="3" t="n"/>
       <c r="I318" s="3" t="n"/>
       <c r="J318" s="3" t="n"/>
-      <c r="K318" s="3" t="n"/>
+      <c r="K318" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="L318" s="3" t="n"/>
       <c r="M318" s="3" t="n"/>
       <c r="N318" s="3" t="n"/>
-      <c r="O318" s="3" t="n"/>
+      <c r="O318" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="P318" s="3" t="n"/>
       <c r="Q318" s="3" t="n"/>
       <c r="R318" s="3" t="n"/>
@@ -12788,7 +12744,11 @@
           <t>MLU</t>
         </is>
       </c>
-      <c r="C319" s="3" t="n"/>
+      <c r="C319" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D319" s="3" t="n"/>
       <c r="E319" s="3" t="n"/>
       <c r="F319" s="3" t="n"/>
@@ -12824,13 +12784,29 @@
       <c r="D320" s="3" t="n"/>
       <c r="E320" s="3" t="n"/>
       <c r="F320" s="3" t="n"/>
-      <c r="G320" s="3" t="n"/>
+      <c r="G320" s="3" t="inlineStr">
+        <is>
+          <t>LEX,PV</t>
+        </is>
+      </c>
       <c r="H320" s="3" t="n"/>
-      <c r="I320" s="3" t="n"/>
+      <c r="I320" s="3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="J320" s="3" t="n"/>
       <c r="K320" s="3" t="n"/>
-      <c r="L320" s="3" t="n"/>
-      <c r="M320" s="3" t="n"/>
+      <c r="L320" s="3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="M320" s="3" t="inlineStr">
+        <is>
+          <t>LEX,PV</t>
+        </is>
+      </c>
       <c r="N320" s="3" t="n"/>
       <c r="O320" s="3" t="n"/>
       <c r="P320" s="3" t="n"/>
@@ -12939,6 +12915,266 @@
       <c r="W323" s="3" t="n"/>
       <c r="X323" s="3" t="n"/>
     </row>
+    <row r="324">
+      <c r="A324" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="B324" s="2" t="inlineStr">
+        <is>
+          <t>Utt</t>
+        </is>
+      </c>
+      <c r="C324" s="2" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="D324" s="2" t="inlineStr">
+        <is>
+          <t>uh</t>
+        </is>
+      </c>
+      <c r="E324" s="2" t="inlineStr">
+        <is>
+          <t>uh</t>
+        </is>
+      </c>
+      <c r="F324" s="2" t="inlineStr">
+        <is>
+          <t>uh</t>
+        </is>
+      </c>
+      <c r="G324" s="2" t="inlineStr">
+        <is>
+          <t>sorry</t>
+        </is>
+      </c>
+      <c r="H324" s="2" t="n"/>
+      <c r="I324" s="2" t="n"/>
+      <c r="J324" s="2" t="n"/>
+      <c r="K324" s="2" t="n"/>
+      <c r="L324" s="2" t="n"/>
+      <c r="M324" s="2" t="n"/>
+      <c r="N324" s="2" t="n"/>
+      <c r="O324" s="2" t="n"/>
+      <c r="P324" s="2" t="n"/>
+      <c r="Q324" s="2" t="n"/>
+      <c r="R324" s="2" t="n"/>
+      <c r="S324" s="2" t="n"/>
+      <c r="T324" s="2" t="n"/>
+      <c r="U324" s="2" t="n"/>
+      <c r="V324" s="2" t="n"/>
+      <c r="W324" s="2" t="n"/>
+      <c r="X324" s="2" t="n"/>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>47</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>SampleGrootte</t>
+        </is>
+      </c>
+      <c r="C325" s="3" t="n"/>
+      <c r="D325" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E325" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F325" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G325" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H325" s="3" t="n"/>
+      <c r="I325" s="3" t="n"/>
+      <c r="J325" s="3" t="n"/>
+      <c r="K325" s="3" t="n"/>
+      <c r="L325" s="3" t="n"/>
+      <c r="M325" s="3" t="n"/>
+      <c r="N325" s="3" t="n"/>
+      <c r="O325" s="3" t="n"/>
+      <c r="P325" s="3" t="n"/>
+      <c r="Q325" s="3" t="n"/>
+      <c r="R325" s="3" t="n"/>
+      <c r="S325" s="3" t="n"/>
+      <c r="T325" s="3" t="n"/>
+      <c r="U325" s="3" t="n"/>
+      <c r="V325" s="3" t="n"/>
+      <c r="W325" s="3" t="n"/>
+      <c r="X325" s="3" t="n"/>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>47</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>MLU</t>
+        </is>
+      </c>
+      <c r="C326" s="3" t="n"/>
+      <c r="D326" s="3" t="n"/>
+      <c r="E326" s="3" t="n"/>
+      <c r="F326" s="3" t="n"/>
+      <c r="G326" s="3" t="n"/>
+      <c r="H326" s="3" t="n"/>
+      <c r="I326" s="3" t="n"/>
+      <c r="J326" s="3" t="n"/>
+      <c r="K326" s="3" t="n"/>
+      <c r="L326" s="3" t="n"/>
+      <c r="M326" s="3" t="n"/>
+      <c r="N326" s="3" t="n"/>
+      <c r="O326" s="3" t="n"/>
+      <c r="P326" s="3" t="n"/>
+      <c r="Q326" s="3" t="n"/>
+      <c r="R326" s="3" t="n"/>
+      <c r="S326" s="3" t="n"/>
+      <c r="T326" s="3" t="n"/>
+      <c r="U326" s="3" t="n"/>
+      <c r="V326" s="3" t="n"/>
+      <c r="W326" s="3" t="n"/>
+      <c r="X326" s="3" t="n"/>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>47</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Taalmaat</t>
+        </is>
+      </c>
+      <c r="C327" s="3" t="n"/>
+      <c r="D327" s="3" t="n"/>
+      <c r="E327" s="3" t="n"/>
+      <c r="F327" s="3" t="n"/>
+      <c r="G327" s="3" t="n"/>
+      <c r="H327" s="3" t="n"/>
+      <c r="I327" s="3" t="n"/>
+      <c r="J327" s="3" t="n"/>
+      <c r="K327" s="3" t="n"/>
+      <c r="L327" s="3" t="n"/>
+      <c r="M327" s="3" t="n"/>
+      <c r="N327" s="3" t="n"/>
+      <c r="O327" s="3" t="n"/>
+      <c r="P327" s="3" t="n"/>
+      <c r="Q327" s="3" t="n"/>
+      <c r="R327" s="3" t="n"/>
+      <c r="S327" s="3" t="n"/>
+      <c r="T327" s="3" t="n"/>
+      <c r="U327" s="3" t="n"/>
+      <c r="V327" s="3" t="n"/>
+      <c r="W327" s="3" t="n"/>
+      <c r="X327" s="3" t="n"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>47</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Lemma</t>
+        </is>
+      </c>
+      <c r="C328" s="3" t="n"/>
+      <c r="D328" s="3" t="n"/>
+      <c r="E328" s="3" t="n"/>
+      <c r="F328" s="3" t="n"/>
+      <c r="G328" s="3" t="n"/>
+      <c r="H328" s="3" t="n"/>
+      <c r="I328" s="3" t="n"/>
+      <c r="J328" s="3" t="n"/>
+      <c r="K328" s="3" t="n"/>
+      <c r="L328" s="3" t="n"/>
+      <c r="M328" s="3" t="n"/>
+      <c r="N328" s="3" t="n"/>
+      <c r="O328" s="3" t="n"/>
+      <c r="P328" s="3" t="n"/>
+      <c r="Q328" s="3" t="n"/>
+      <c r="R328" s="3" t="n"/>
+      <c r="S328" s="3" t="n"/>
+      <c r="T328" s="3" t="n"/>
+      <c r="U328" s="3" t="n"/>
+      <c r="V328" s="3" t="n"/>
+      <c r="W328" s="3" t="n"/>
+      <c r="X328" s="3" t="n"/>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>47</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Grammaticale fout</t>
+        </is>
+      </c>
+      <c r="C329" s="3" t="n"/>
+      <c r="D329" s="3" t="n"/>
+      <c r="E329" s="3" t="n"/>
+      <c r="F329" s="3" t="n"/>
+      <c r="G329" s="3" t="n"/>
+      <c r="H329" s="3" t="n"/>
+      <c r="I329" s="3" t="n"/>
+      <c r="J329" s="3" t="n"/>
+      <c r="K329" s="3" t="n"/>
+      <c r="L329" s="3" t="n"/>
+      <c r="M329" s="3" t="n"/>
+      <c r="N329" s="3" t="n"/>
+      <c r="O329" s="3" t="n"/>
+      <c r="P329" s="3" t="n"/>
+      <c r="Q329" s="3" t="n"/>
+      <c r="R329" s="3" t="n"/>
+      <c r="S329" s="3" t="n"/>
+      <c r="T329" s="3" t="n"/>
+      <c r="U329" s="3" t="n"/>
+      <c r="V329" s="3" t="n"/>
+      <c r="W329" s="3" t="n"/>
+      <c r="X329" s="3" t="n"/>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>47</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="C330" s="3" t="n"/>
+      <c r="D330" s="3" t="n"/>
+      <c r="E330" s="3" t="n"/>
+      <c r="F330" s="3" t="n"/>
+      <c r="G330" s="3" t="n"/>
+      <c r="H330" s="3" t="n"/>
+      <c r="I330" s="3" t="n"/>
+      <c r="J330" s="3" t="n"/>
+      <c r="K330" s="3" t="n"/>
+      <c r="L330" s="3" t="n"/>
+      <c r="M330" s="3" t="n"/>
+      <c r="N330" s="3" t="n"/>
+      <c r="O330" s="3" t="n"/>
+      <c r="P330" s="3" t="n"/>
+      <c r="Q330" s="3" t="n"/>
+      <c r="R330" s="3" t="n"/>
+      <c r="S330" s="3" t="n"/>
+      <c r="T330" s="3" t="n"/>
+      <c r="U330" s="3" t="n"/>
+      <c r="V330" s="3" t="n"/>
+      <c r="W330" s="3" t="n"/>
+      <c r="X330" s="3" t="n"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>